<commit_message>
[CSTPER-262] Allow to reference objects by their business identifiers in the bulk import
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/create-publication-with-authority.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/create-publication-with-authority.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">ROW-ID::2</t>
   </si>
   <si>
-    <t xml:space="preserve">Author1::authority1</t>
+    <t xml:space="preserve">Author1$$authority1</t>
   </si>
   <si>
     <t xml:space="preserve">OrgUnit1</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">Author2</t>
   </si>
   <si>
-    <t xml:space="preserve">OrgUnit2::authority2::400</t>
+    <t xml:space="preserve">OrgUnit2$$authority2$$400</t>
   </si>
 </sst>
 </file>
@@ -177,7 +177,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.81"/>
   </cols>
@@ -215,10 +215,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.38"/>

</xml_diff>

<commit_message>
[CSTPER-451] Import via XLS should offer stop in workspace, send to workflow and skip workflow
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/create-publication-with-authority.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/create-publication-with-authority.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -29,7 +29,22 @@
     <t xml:space="preserve">ACTION</t>
   </si>
   <si>
+    <t xml:space="preserve">dc.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc.date.issued</t>
+  </si>
+  <si>
     <t xml:space="preserve">ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Publication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article</t>
   </si>
   <si>
     <t xml:space="preserve">PARENT-ID</t>
@@ -60,8 +75,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -141,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,6 +167,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -171,15 +191,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,11 +211,28 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>43831</v>
       </c>
     </row>
   </sheetData>
@@ -214,11 +253,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.38"/>
@@ -227,35 +266,35 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>